<commit_message>
2 skritt frem, 1 tilbake
</commit_message>
<xml_diff>
--- a/Input_data_testkode.xlsx
+++ b/Input_data_testkode.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b737bfa27afa4358/Dokumenter/10. semester/Til master/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b737bfa27afa4358/Dokumenter/10. semester/Til master/Master_multi_stage_v1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{108884CD-89E4-4EE9-8121-A78EE75AA4B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E1B135D-72F9-4E2B-8A36-D95C0F5A9C16}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{108884CD-89E4-4EE9-8121-A78EE75AA4B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E5A54D3-6347-48B2-AE93-1DB163E80775}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="26" activeTab="31" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="13" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Par_ActivationFactor_Dwn_Reg" sheetId="1" r:id="rId1"/>
@@ -57,13 +57,22 @@
     <sheet name="Subset_ShiftableLoadForEC" sheetId="47" r:id="rId42"/>
     <sheet name="Subset_ECToTech" sheetId="40" r:id="rId43"/>
     <sheet name="Subset_TechToEC" sheetId="41" r:id="rId44"/>
-    <sheet name="Set_parent_nodes" sheetId="51" r:id="rId45"/>
+    <sheet name="Set_Parent_Node" sheetId="51" r:id="rId45"/>
     <sheet name="Set_parent_coupling" sheetId="52" r:id="rId46"/>
     <sheet name="Subset_Plan_Nodes" sheetId="48" r:id="rId47"/>
     <sheet name="Subset_ID_Nodes" sheetId="49" r:id="rId48"/>
     <sheet name="Subset_RT_Nodes" sheetId="50" r:id="rId49"/>
-    <sheet name="Set_Operational_Mode" sheetId="53" r:id="rId50"/>
-    <sheet name="Set_Strategic_Periods" sheetId="54" r:id="rId51"/>
+    <sheet name="Set_Mode_of_Operation" sheetId="53" r:id="rId50"/>
+    <sheet name="Par_BatteryCost" sheetId="55" r:id="rId51"/>
+    <sheet name="Par_CostImbalance" sheetId="56" r:id="rId52"/>
+    <sheet name="Par_SpotPrice" sheetId="57" r:id="rId53"/>
+    <sheet name="Par_IntradayPrice" sheetId="58" r:id="rId54"/>
+    <sheet name="Par_RK_UpPrice" sheetId="59" r:id="rId55"/>
+    <sheet name="Par_RK_DwnPrice" sheetId="60" r:id="rId56"/>
+    <sheet name="Set_Strategic_Periods" sheetId="54" r:id="rId57"/>
+    <sheet name="Par_Max_Capex_tec" sheetId="61" r:id="rId58"/>
+    <sheet name="Par_Max_Capex_bat" sheetId="62" r:id="rId59"/>
+    <sheet name="Par_Max_Carbon_Emission" sheetId="63" r:id="rId60"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">Par_ExportCost!$A$3:$D$59</definedName>
@@ -87,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2098" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2151" uniqueCount="135">
   <si>
     <t>Benevning:</t>
   </si>
@@ -813,7 +822,22 @@
     <t>Obs: antatt at Gas Boiler LT og MT, samt Electric Boiler LT og MT har samme cost expansion. Må ellers legge til dimensjon av fuel eller modus</t>
   </si>
   <si>
-    <t>15+A49:D71</t>
+    <t>CostImbalance</t>
+  </si>
+  <si>
+    <t>SpotPrice</t>
+  </si>
+  <si>
+    <t>IntradayPrice</t>
+  </si>
+  <si>
+    <t>RKUpPrice</t>
+  </si>
+  <si>
+    <t>Capex</t>
+  </si>
+  <si>
+    <t>Max Carbon E</t>
   </si>
 </sst>
 </file>
@@ -1459,7 +1483,7 @@
       </c>
       <c r="C4" s="11">
         <f ca="1">RANDBETWEEN(0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1483,7 +1507,7 @@
       </c>
       <c r="C6" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1507,7 +1531,7 @@
       </c>
       <c r="C8" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1591,7 +1615,7 @@
       </c>
       <c r="C15" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1615,7 +1639,7 @@
       </c>
       <c r="C17" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1627,7 +1651,7 @@
       </c>
       <c r="C18" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1639,7 +1663,7 @@
       </c>
       <c r="C19" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1651,7 +1675,7 @@
       </c>
       <c r="C20" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1675,7 +1699,7 @@
       </c>
       <c r="C22" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1723,7 +1747,7 @@
       </c>
       <c r="C26" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1735,7 +1759,7 @@
       </c>
       <c r="C27" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1747,7 +1771,7 @@
       </c>
       <c r="C28" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1759,7 +1783,7 @@
       </c>
       <c r="C29" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1795,7 +1819,7 @@
       </c>
       <c r="C32" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1807,7 +1831,7 @@
       </c>
       <c r="C33" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1855,7 +1879,7 @@
       </c>
       <c r="C37" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1867,7 +1891,7 @@
       </c>
       <c r="C38" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1891,7 +1915,7 @@
       </c>
       <c r="C40" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1903,7 +1927,7 @@
       </c>
       <c r="C41" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1927,7 +1951,7 @@
       </c>
       <c r="C43" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1939,7 +1963,7 @@
       </c>
       <c r="C44" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1963,7 +1987,7 @@
       </c>
       <c r="C46" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -3098,8 +3122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:N558"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B48"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3575,7 +3599,7 @@
         <v>12</v>
       </c>
       <c r="D29">
-        <f t="shared" ref="D29:D51" si="0">D5*0.8</f>
+        <f t="shared" ref="D29:D48" si="0">D5*0.8</f>
         <v>2.7680000000000002</v>
       </c>
       <c r="K29" s="5"/>
@@ -3893,7 +3917,7 @@
         <v>8.895999999999999</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>1</v>
       </c>
@@ -3907,7 +3931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>1</v>
       </c>
@@ -3921,7 +3945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>1</v>
       </c>
@@ -3935,7 +3959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2</v>
       </c>
@@ -3949,7 +3973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2</v>
       </c>
@@ -3963,7 +3987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2</v>
       </c>
@@ -3976,11 +4000,8 @@
       <c r="D54">
         <v>0</v>
       </c>
-      <c r="G54" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>3</v>
       </c>
@@ -3994,7 +4015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>3</v>
       </c>
@@ -4008,7 +4029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>3</v>
       </c>
@@ -4022,7 +4043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>4</v>
       </c>
@@ -4036,7 +4057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>4</v>
       </c>
@@ -4050,7 +4071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>4</v>
       </c>
@@ -4064,7 +4085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>5</v>
       </c>
@@ -4078,7 +4099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>5</v>
       </c>
@@ -4092,7 +4113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>5</v>
       </c>
@@ -4106,7 +4127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>6</v>
       </c>
@@ -15412,8 +15433,8 @@
         <v>2</v>
       </c>
       <c r="C5" s="11">
-        <f t="shared" ref="C5:C68" ca="1" si="0">RANDBETWEEN(0,1)</f>
-        <v>0</v>
+        <f t="shared" ref="C5:C48" ca="1" si="0">RANDBETWEEN(0,1)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -15461,7 +15482,7 @@
       </c>
       <c r="C9" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -15473,7 +15494,7 @@
       </c>
       <c r="C10" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -15497,7 +15518,7 @@
       </c>
       <c r="C12" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -15509,7 +15530,7 @@
       </c>
       <c r="C13" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -15521,7 +15542,7 @@
       </c>
       <c r="C14" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -15533,7 +15554,7 @@
       </c>
       <c r="C15" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -15557,7 +15578,7 @@
       </c>
       <c r="C17" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -15569,7 +15590,7 @@
       </c>
       <c r="C18" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -15629,7 +15650,7 @@
       </c>
       <c r="C23" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -15665,7 +15686,7 @@
       </c>
       <c r="C26" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -15677,7 +15698,7 @@
       </c>
       <c r="C27" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -15689,7 +15710,7 @@
       </c>
       <c r="C28" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -15713,7 +15734,7 @@
       </c>
       <c r="C30" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -15749,7 +15770,7 @@
       </c>
       <c r="C33" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -15761,7 +15782,7 @@
       </c>
       <c r="C34" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -15773,7 +15794,7 @@
       </c>
       <c r="C35" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -15785,7 +15806,7 @@
       </c>
       <c r="C36" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -15809,7 +15830,7 @@
       </c>
       <c r="C38" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -15845,7 +15866,7 @@
       </c>
       <c r="C41" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -15857,7 +15878,7 @@
       </c>
       <c r="C42" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -15869,7 +15890,7 @@
       </c>
       <c r="C43" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -15881,7 +15902,7 @@
       </c>
       <c r="C44" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -15893,7 +15914,7 @@
       </c>
       <c r="C45" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -15917,7 +15938,7 @@
       </c>
       <c r="C47" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -15929,7 +15950,7 @@
       </c>
       <c r="C48" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="3:3" x14ac:dyDescent="0.25">
@@ -19804,7 +19825,7 @@
         <v>49</v>
       </c>
       <c r="D269">
-        <f t="shared" ref="D269:D291" si="1">D221*1.2</f>
+        <f t="shared" ref="D269:D273" si="1">D221*1.2</f>
         <v>180.18</v>
       </c>
     </row>
@@ -21269,7 +21290,7 @@
       </c>
       <c r="C4" s="28">
         <f ca="1">RANDBETWEEN(0,30)</f>
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -21281,7 +21302,7 @@
       </c>
       <c r="C5" s="28">
         <f t="shared" ref="C5:C48" ca="1" si="0">RANDBETWEEN(0,30)</f>
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -21293,7 +21314,7 @@
       </c>
       <c r="C6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -21305,7 +21326,7 @@
       </c>
       <c r="C7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -21317,7 +21338,7 @@
       </c>
       <c r="C8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -21329,7 +21350,7 @@
       </c>
       <c r="C9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -21353,7 +21374,7 @@
       </c>
       <c r="C11" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -21365,7 +21386,7 @@
       </c>
       <c r="C12" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -21377,7 +21398,7 @@
       </c>
       <c r="C13" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -21389,7 +21410,7 @@
       </c>
       <c r="C14" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -21401,7 +21422,7 @@
       </c>
       <c r="C15" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -21413,7 +21434,7 @@
       </c>
       <c r="C16" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -21425,7 +21446,7 @@
       </c>
       <c r="C17" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -21449,7 +21470,7 @@
       </c>
       <c r="C19" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -21461,7 +21482,7 @@
       </c>
       <c r="C20" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -21473,7 +21494,7 @@
       </c>
       <c r="C21" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -21485,7 +21506,7 @@
       </c>
       <c r="C22" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -21497,7 +21518,7 @@
       </c>
       <c r="C23" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -21509,7 +21530,7 @@
       </c>
       <c r="C24" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -21521,7 +21542,7 @@
       </c>
       <c r="C25" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="D25" s="3"/>
     </row>
@@ -21534,7 +21555,7 @@
       </c>
       <c r="C26" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -21546,7 +21567,7 @@
       </c>
       <c r="C27" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -21558,7 +21579,7 @@
       </c>
       <c r="C28" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -21570,7 +21591,7 @@
       </c>
       <c r="C29" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -21582,7 +21603,7 @@
       </c>
       <c r="C30" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -21594,7 +21615,7 @@
       </c>
       <c r="C31" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -21606,7 +21627,7 @@
       </c>
       <c r="C32" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -21618,7 +21639,7 @@
       </c>
       <c r="C33" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -21630,7 +21651,7 @@
       </c>
       <c r="C34" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -21642,7 +21663,7 @@
       </c>
       <c r="C35" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -21654,7 +21675,7 @@
       </c>
       <c r="C36" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -21666,7 +21687,7 @@
       </c>
       <c r="C37" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -21678,7 +21699,7 @@
       </c>
       <c r="C38" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -21690,7 +21711,7 @@
       </c>
       <c r="C39" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>25</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -21714,7 +21735,7 @@
       </c>
       <c r="C41" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -21726,7 +21747,7 @@
       </c>
       <c r="C42" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -21738,7 +21759,7 @@
       </c>
       <c r="C43" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -21750,7 +21771,7 @@
       </c>
       <c r="C44" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -21762,7 +21783,7 @@
       </c>
       <c r="C45" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>21</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -21774,7 +21795,7 @@
       </c>
       <c r="C46" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -21786,7 +21807,7 @@
       </c>
       <c r="C47" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -21798,7 +21819,7 @@
       </c>
       <c r="C48" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -22172,7 +22193,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <dimension ref="A3:A9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
@@ -22226,7 +22247,7 @@
   <dimension ref="A3:A16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A3" sqref="A3:A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22565,7 +22586,7 @@
   <dimension ref="A3:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22797,7 +22818,7 @@
       </c>
       <c r="C4" s="28">
         <f ca="1">RANDBETWEEN(0,30)</f>
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="H4" s="32"/>
       <c r="I4" s="32"/>
@@ -22816,7 +22837,7 @@
       </c>
       <c r="C5" s="28">
         <f t="shared" ref="C5:C48" ca="1" si="0">RANDBETWEEN(0,30)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H5" s="32"/>
       <c r="I5" s="34"/>
@@ -22835,7 +22856,7 @@
       </c>
       <c r="C6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="H6" s="32"/>
       <c r="I6" s="34"/>
@@ -22854,7 +22875,7 @@
       </c>
       <c r="C7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="H7" s="32"/>
       <c r="I7" s="34"/>
@@ -22873,7 +22894,7 @@
       </c>
       <c r="C8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="H8" s="32"/>
       <c r="I8" s="34"/>
@@ -22892,7 +22913,7 @@
       </c>
       <c r="C9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="H9" s="32"/>
       <c r="I9" s="34"/>
@@ -22911,7 +22932,7 @@
       </c>
       <c r="C10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="H10" s="32"/>
       <c r="I10" s="34"/>
@@ -22930,7 +22951,7 @@
       </c>
       <c r="C11" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="H11" s="32"/>
       <c r="I11" s="34"/>
@@ -22949,7 +22970,7 @@
       </c>
       <c r="C12" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="H12" s="32"/>
       <c r="I12" s="34"/>
@@ -22968,7 +22989,7 @@
       </c>
       <c r="C13" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="H13" s="32"/>
       <c r="I13" s="34"/>
@@ -22987,7 +23008,7 @@
       </c>
       <c r="C14" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="H14" s="32"/>
       <c r="I14" s="34"/>
@@ -23006,7 +23027,7 @@
       </c>
       <c r="C15" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="H15" s="32"/>
       <c r="I15" s="34"/>
@@ -23025,7 +23046,7 @@
       </c>
       <c r="C16" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="H16" s="32"/>
       <c r="I16" s="34"/>
@@ -23044,7 +23065,7 @@
       </c>
       <c r="C17" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="H17" s="32"/>
       <c r="I17" s="34"/>
@@ -23063,7 +23084,7 @@
       </c>
       <c r="C18" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="H18" s="32"/>
       <c r="I18" s="34"/>
@@ -23082,7 +23103,7 @@
       </c>
       <c r="C19" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="H19" s="32"/>
       <c r="I19" s="34"/>
@@ -23101,7 +23122,7 @@
       </c>
       <c r="C20" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="H20" s="32"/>
       <c r="I20" s="34"/>
@@ -23120,7 +23141,7 @@
       </c>
       <c r="C21" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="H21" s="32"/>
       <c r="I21" s="34"/>
@@ -23139,7 +23160,7 @@
       </c>
       <c r="C22" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="H22" s="32"/>
       <c r="I22" s="34"/>
@@ -23158,7 +23179,7 @@
       </c>
       <c r="C23" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="H23" s="32"/>
       <c r="I23" s="34"/>
@@ -23177,7 +23198,7 @@
       </c>
       <c r="C24" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="H24" s="32"/>
       <c r="I24" s="34"/>
@@ -23196,7 +23217,7 @@
       </c>
       <c r="C25" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H25" s="32"/>
       <c r="I25" s="34"/>
@@ -23215,7 +23236,7 @@
       </c>
       <c r="C26" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H26" s="32"/>
       <c r="I26" s="34"/>
@@ -23234,7 +23255,7 @@
       </c>
       <c r="C27" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="H27" s="32"/>
       <c r="I27" s="34"/>
@@ -23253,7 +23274,7 @@
       </c>
       <c r="C28" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="H28" s="32"/>
       <c r="I28" s="33"/>
@@ -23272,7 +23293,7 @@
       </c>
       <c r="C29" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
@@ -23290,7 +23311,7 @@
       </c>
       <c r="C30" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
@@ -23308,7 +23329,7 @@
       </c>
       <c r="C31" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
@@ -23326,7 +23347,7 @@
       </c>
       <c r="C32" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
@@ -23344,7 +23365,7 @@
       </c>
       <c r="C33" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
@@ -23362,7 +23383,7 @@
       </c>
       <c r="C34" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
@@ -23380,7 +23401,7 @@
       </c>
       <c r="C35" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
@@ -23398,7 +23419,7 @@
       </c>
       <c r="C36" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
@@ -23410,7 +23431,7 @@
       </c>
       <c r="C37" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
@@ -23434,7 +23455,7 @@
       </c>
       <c r="C39" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
@@ -23446,7 +23467,7 @@
       </c>
       <c r="C40" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
@@ -23458,7 +23479,7 @@
       </c>
       <c r="C41" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
@@ -23470,7 +23491,7 @@
       </c>
       <c r="C42" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>28</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
@@ -23482,7 +23503,7 @@
       </c>
       <c r="C43" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
@@ -23494,7 +23515,7 @@
       </c>
       <c r="C44" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
@@ -23506,7 +23527,7 @@
       </c>
       <c r="C45" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
@@ -23518,7 +23539,7 @@
       </c>
       <c r="C46" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
@@ -23530,7 +23551,7 @@
       </c>
       <c r="C47" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
@@ -23542,7 +23563,7 @@
       </c>
       <c r="C48" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -24239,7 +24260,7 @@
   <dimension ref="A3:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="A4" sqref="A4:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24297,7 +24318,7 @@
   <dimension ref="A3:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24611,7 +24632,7 @@
       </c>
       <c r="C4" s="28">
         <f ca="1">RANDBETWEEN(0,30)</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
@@ -24634,7 +24655,7 @@
       </c>
       <c r="C5" s="28">
         <f t="shared" ref="C5:C48" ca="1" si="0">RANDBETWEEN(0,30)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
@@ -24657,7 +24678,7 @@
       </c>
       <c r="C6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
@@ -24680,7 +24701,7 @@
       </c>
       <c r="C7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
@@ -24703,7 +24724,7 @@
       </c>
       <c r="C8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
@@ -24726,7 +24747,7 @@
       </c>
       <c r="C9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
@@ -24749,7 +24770,7 @@
       </c>
       <c r="C10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
@@ -24795,7 +24816,7 @@
       </c>
       <c r="C12" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
@@ -24818,7 +24839,7 @@
       </c>
       <c r="C13" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
@@ -24841,7 +24862,7 @@
       </c>
       <c r="C14" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
@@ -24864,7 +24885,7 @@
       </c>
       <c r="C15" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
@@ -24887,7 +24908,7 @@
       </c>
       <c r="C16" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
@@ -24910,7 +24931,7 @@
       </c>
       <c r="C17" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
@@ -24933,7 +24954,7 @@
       </c>
       <c r="C18" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
@@ -24956,7 +24977,7 @@
       </c>
       <c r="C19" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
@@ -24979,7 +25000,7 @@
       </c>
       <c r="C20" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
@@ -25002,7 +25023,7 @@
       </c>
       <c r="C21" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
@@ -25048,7 +25069,7 @@
       </c>
       <c r="C23" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
@@ -25071,7 +25092,7 @@
       </c>
       <c r="C24" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
@@ -25094,7 +25115,7 @@
       </c>
       <c r="C25" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
@@ -25117,7 +25138,7 @@
       </c>
       <c r="C26" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
@@ -25140,7 +25161,7 @@
       </c>
       <c r="C27" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E27" s="5"/>
       <c r="H27" s="5"/>
@@ -25164,7 +25185,7 @@
       </c>
       <c r="C28" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
@@ -25210,7 +25231,7 @@
       </c>
       <c r="C30" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
@@ -25233,7 +25254,7 @@
       </c>
       <c r="C31" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
@@ -25256,7 +25277,7 @@
       </c>
       <c r="C32" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
@@ -25279,7 +25300,7 @@
       </c>
       <c r="C33" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
@@ -25302,7 +25323,7 @@
       </c>
       <c r="C34" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
@@ -25325,7 +25346,7 @@
       </c>
       <c r="C35" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
@@ -25337,7 +25358,7 @@
       </c>
       <c r="C36" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
@@ -25349,7 +25370,7 @@
       </c>
       <c r="C37" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
@@ -25361,7 +25382,7 @@
       </c>
       <c r="C38" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
@@ -25373,7 +25394,7 @@
       </c>
       <c r="C39" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
@@ -25385,7 +25406,7 @@
       </c>
       <c r="C40" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
@@ -25397,7 +25418,7 @@
       </c>
       <c r="C41" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
@@ -25409,7 +25430,7 @@
       </c>
       <c r="C42" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
@@ -25421,7 +25442,7 @@
       </c>
       <c r="C43" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
@@ -25433,7 +25454,7 @@
       </c>
       <c r="C44" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
@@ -25445,7 +25466,7 @@
       </c>
       <c r="C45" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
@@ -25457,7 +25478,7 @@
       </c>
       <c r="C46" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>26</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
@@ -25469,7 +25490,7 @@
       </c>
       <c r="C47" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
@@ -25481,7 +25502,7 @@
       </c>
       <c r="C48" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -25528,6 +25549,1803 @@
 </file>
 
 <file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7815BD0D-D4C8-43C3-B5E1-419A131BCC6A}">
+  <dimension ref="A3:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>101</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>102</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>103</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B076616-024E-4AB1-B79B-88202D242CCF}">
+  <dimension ref="A3:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84C73887-EC92-4CCB-BB63-90308D4E3D86}">
+  <dimension ref="A3:C48"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:C48"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="28">
+        <v>3.54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" s="28">
+        <v>3.46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6" s="28">
+        <v>4.28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="28">
+        <v>4.82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" s="28">
+        <v>3.59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9" s="28">
+        <v>3.59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="28">
+        <v>5.09</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" s="28">
+        <v>10.130000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12" s="28">
+        <v>12.01</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" s="28">
+        <v>14.41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" s="28">
+        <v>21.22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15" s="28">
+        <v>21.63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" s="28">
+        <v>21.01</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>5</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" s="28">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18" s="28">
+        <v>20.98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>6</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" s="28">
+        <v>21.43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>6</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20" s="28">
+        <v>19.79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>6</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21" s="28">
+        <v>18.02</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>7</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" s="28">
+        <v>13.82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>7</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23" s="28">
+        <v>11.63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>7</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24" s="28">
+        <v>11.12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>8</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" s="28">
+        <v>10.4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>8</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26" s="28">
+        <v>5.17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>8</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27" s="28">
+        <v>4.88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>9</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <f>C4*0.8</f>
+        <v>2.8320000000000003</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>9</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <f t="shared" ref="C29:C48" si="0">C5*0.8</f>
+        <v>2.7680000000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>9</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>3.4240000000000004</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>10</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>3.8560000000000003</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>10</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>2.8719999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>10</v>
+      </c>
+      <c r="B33">
+        <v>3</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>2.8719999999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>11</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>4.0720000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>11</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>8.104000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>11</v>
+      </c>
+      <c r="B36">
+        <v>3</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>9.6080000000000005</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>12</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="0"/>
+        <v>11.528</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>12</v>
+      </c>
+      <c r="B38">
+        <v>2</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="0"/>
+        <v>16.975999999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>12</v>
+      </c>
+      <c r="B39">
+        <v>3</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="0"/>
+        <v>17.303999999999998</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>13</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>16.808000000000003</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>13</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="0"/>
+        <v>16.8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>13</v>
+      </c>
+      <c r="B42">
+        <v>3</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="0"/>
+        <v>16.784000000000002</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>14</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="0"/>
+        <v>17.144000000000002</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>14</v>
+      </c>
+      <c r="B44">
+        <v>2</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="0"/>
+        <v>15.832000000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>14</v>
+      </c>
+      <c r="B45">
+        <v>3</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="0"/>
+        <v>14.416</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>15</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="0"/>
+        <v>11.056000000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>15</v>
+      </c>
+      <c r="B47">
+        <v>2</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="0"/>
+        <v>9.3040000000000003</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>15</v>
+      </c>
+      <c r="B48">
+        <v>3</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="0"/>
+        <v>8.895999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A34583D8-B68B-48CF-AB50-5E1E48B2C8C1}">
+  <dimension ref="A3:C48"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:C48"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="28">
+        <v>3.54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" s="28">
+        <v>3.46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6" s="28">
+        <v>4.28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="28">
+        <v>4.82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" s="28">
+        <v>3.59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9" s="28">
+        <v>3.59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="28">
+        <v>5.09</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" s="28">
+        <v>10.130000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12" s="28">
+        <v>12.01</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" s="28">
+        <v>14.41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" s="28">
+        <v>21.22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15" s="28">
+        <v>21.63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" s="28">
+        <v>21.01</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>5</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" s="28">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18" s="28">
+        <v>20.98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>6</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" s="28">
+        <v>21.43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>6</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20" s="28">
+        <v>19.79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>6</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21" s="28">
+        <v>18.02</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>7</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" s="28">
+        <v>13.82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>7</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23" s="28">
+        <v>11.63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>7</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24" s="28">
+        <v>11.12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>8</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" s="28">
+        <v>10.4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>8</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26" s="28">
+        <v>5.17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>8</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27" s="28">
+        <v>4.88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>9</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <f>C4*0.8</f>
+        <v>2.8320000000000003</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>9</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <f t="shared" ref="C29:C48" si="0">C5*0.8</f>
+        <v>2.7680000000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>9</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>3.4240000000000004</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>10</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>3.8560000000000003</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>10</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>2.8719999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>10</v>
+      </c>
+      <c r="B33">
+        <v>3</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>2.8719999999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>11</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>4.0720000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>11</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>8.104000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>11</v>
+      </c>
+      <c r="B36">
+        <v>3</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>9.6080000000000005</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>12</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="0"/>
+        <v>11.528</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>12</v>
+      </c>
+      <c r="B38">
+        <v>2</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="0"/>
+        <v>16.975999999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>12</v>
+      </c>
+      <c r="B39">
+        <v>3</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="0"/>
+        <v>17.303999999999998</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>13</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>16.808000000000003</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>13</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="0"/>
+        <v>16.8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>13</v>
+      </c>
+      <c r="B42">
+        <v>3</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="0"/>
+        <v>16.784000000000002</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>14</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="0"/>
+        <v>17.144000000000002</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>14</v>
+      </c>
+      <c r="B44">
+        <v>2</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="0"/>
+        <v>15.832000000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>14</v>
+      </c>
+      <c r="B45">
+        <v>3</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="0"/>
+        <v>14.416</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>15</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="0"/>
+        <v>11.056000000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>15</v>
+      </c>
+      <c r="B47">
+        <v>2</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="0"/>
+        <v>9.3040000000000003</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>15</v>
+      </c>
+      <c r="B48">
+        <v>3</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="0"/>
+        <v>8.895999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE259879-7F8E-4068-80DD-1A71A9A2E767}">
+  <dimension ref="A3:C48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="28">
+        <v>3.54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" s="28">
+        <v>3.46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6" s="28">
+        <v>4.28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="28">
+        <v>4.82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" s="28">
+        <v>3.59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9" s="28">
+        <v>3.59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="28">
+        <v>5.09</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" s="28">
+        <v>10.130000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12" s="28">
+        <v>12.01</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" s="28">
+        <v>14.41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" s="28">
+        <v>21.22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15" s="28">
+        <v>21.63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" s="28">
+        <v>21.01</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>5</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" s="28">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18" s="28">
+        <v>20.98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>6</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" s="28">
+        <v>21.43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>6</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20" s="28">
+        <v>19.79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>6</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21" s="28">
+        <v>18.02</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>7</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" s="28">
+        <v>13.82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>7</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23" s="28">
+        <v>11.63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>7</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24" s="28">
+        <v>11.12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>8</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" s="28">
+        <v>10.4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>8</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26" s="28">
+        <v>5.17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>8</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27" s="28">
+        <v>4.88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>9</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <f>C4*0.8</f>
+        <v>2.8320000000000003</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>9</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <f t="shared" ref="C29:C48" si="0">C5*0.8</f>
+        <v>2.7680000000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>9</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>3.4240000000000004</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>10</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>3.8560000000000003</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>10</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>2.8719999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>10</v>
+      </c>
+      <c r="B33">
+        <v>3</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>2.8719999999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>11</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>4.0720000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>11</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>8.104000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>11</v>
+      </c>
+      <c r="B36">
+        <v>3</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>9.6080000000000005</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>12</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="0"/>
+        <v>11.528</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>12</v>
+      </c>
+      <c r="B38">
+        <v>2</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="0"/>
+        <v>16.975999999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>12</v>
+      </c>
+      <c r="B39">
+        <v>3</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="0"/>
+        <v>17.303999999999998</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>13</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>16.808000000000003</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>13</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="0"/>
+        <v>16.8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>13</v>
+      </c>
+      <c r="B42">
+        <v>3</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="0"/>
+        <v>16.784000000000002</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>14</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="0"/>
+        <v>17.144000000000002</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>14</v>
+      </c>
+      <c r="B44">
+        <v>2</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="0"/>
+        <v>15.832000000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>14</v>
+      </c>
+      <c r="B45">
+        <v>3</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="0"/>
+        <v>14.416</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>15</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="0"/>
+        <v>11.056000000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>15</v>
+      </c>
+      <c r="B47">
+        <v>2</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="0"/>
+        <v>9.3040000000000003</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>15</v>
+      </c>
+      <c r="B48">
+        <v>3</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="0"/>
+        <v>8.895999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E77D990-D668-4B4C-BC47-633A78174A57}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFD6BE9E-879D-4B2B-94E0-B0F968CE8029}">
   <dimension ref="A3:A4"/>
   <sheetViews>
@@ -25545,6 +27363,250 @@
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79D8A7B4-563D-4ED3-B0E1-BBA90E6A0CD9}">
+  <dimension ref="A3:B14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>125</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43D2A640-3DE1-4626-909C-0B031DDA6CF5}">
+  <dimension ref="A3:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>101</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>102</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>103</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -25602,7 +27664,7 @@
       </c>
       <c r="C4" s="28">
         <f ca="1">RANDBETWEEN(0,30)</f>
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -25614,7 +27676,7 @@
       </c>
       <c r="C5" s="28">
         <f t="shared" ref="C5:C48" ca="1" si="0">RANDBETWEEN(0,30)</f>
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -25626,7 +27688,7 @@
       </c>
       <c r="C6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -25638,7 +27700,7 @@
       </c>
       <c r="C7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -25650,7 +27712,7 @@
       </c>
       <c r="C8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -25662,7 +27724,7 @@
       </c>
       <c r="C9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -25674,7 +27736,7 @@
       </c>
       <c r="C10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -25686,7 +27748,7 @@
       </c>
       <c r="C11" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -25698,7 +27760,7 @@
       </c>
       <c r="C12" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>21</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -25710,7 +27772,7 @@
       </c>
       <c r="C13" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -25722,7 +27784,7 @@
       </c>
       <c r="C14" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -25734,7 +27796,7 @@
       </c>
       <c r="C15" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -25746,7 +27808,7 @@
       </c>
       <c r="C16" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -25758,7 +27820,7 @@
       </c>
       <c r="C17" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -25770,7 +27832,7 @@
       </c>
       <c r="C18" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -25782,7 +27844,7 @@
       </c>
       <c r="C19" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -25806,7 +27868,7 @@
       </c>
       <c r="C21" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -25818,7 +27880,7 @@
       </c>
       <c r="C22" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -25830,7 +27892,7 @@
       </c>
       <c r="C23" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -25842,7 +27904,7 @@
       </c>
       <c r="C24" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -25854,7 +27916,7 @@
       </c>
       <c r="C25" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -25866,7 +27928,7 @@
       </c>
       <c r="C26" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -25878,7 +27940,7 @@
       </c>
       <c r="C27" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -25890,7 +27952,7 @@
       </c>
       <c r="C28" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -25902,7 +27964,7 @@
       </c>
       <c r="C29" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -25914,7 +27976,7 @@
       </c>
       <c r="C30" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -25926,7 +27988,7 @@
       </c>
       <c r="C31" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -25938,7 +28000,7 @@
       </c>
       <c r="C32" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -25950,7 +28012,7 @@
       </c>
       <c r="C33" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>28</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -25962,7 +28024,7 @@
       </c>
       <c r="C34" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -25974,7 +28036,7 @@
       </c>
       <c r="C35" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -25986,7 +28048,7 @@
       </c>
       <c r="C36" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -25998,7 +28060,7 @@
       </c>
       <c r="C37" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -26010,7 +28072,7 @@
       </c>
       <c r="C38" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -26022,7 +28084,7 @@
       </c>
       <c r="C39" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>23</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -26034,7 +28096,7 @@
       </c>
       <c r="C40" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -26046,7 +28108,7 @@
       </c>
       <c r="C41" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -26058,7 +28120,7 @@
       </c>
       <c r="C42" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -26070,7 +28132,7 @@
       </c>
       <c r="C43" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -26082,7 +28144,7 @@
       </c>
       <c r="C44" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -26094,7 +28156,7 @@
       </c>
       <c r="C45" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -26106,7 +28168,7 @@
       </c>
       <c r="C46" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -26118,7 +28180,7 @@
       </c>
       <c r="C47" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -26130,7 +28192,35 @@
       </c>
       <c r="C48" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02D11E0E-41D4-4644-84B7-5D54908DADEE}">
+  <dimension ref="A3:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -29065,7 +31155,7 @@
         <v>15</v>
       </c>
       <c r="D208">
-        <f t="shared" ref="D208:D231" si="0">D184*1.3</f>
+        <f t="shared" ref="D208:D228" si="0">D184*1.3</f>
         <v>0</v>
       </c>
     </row>
@@ -33656,6 +35746,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5caa653f-10d0-46a2-81cc-01cb3798075e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CEBC57C6511F094FB1659D4FD897CA2A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e300c8dce90f4bd359ffe07958d068a6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5caa653f-10d0-46a2-81cc-01cb3798075e" xmlns:ns3="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="947f29ac9f688054ae1e7aaca14544db" ns2:_="" ns3:_="">
     <xsd:import namespace="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
@@ -33856,27 +35966,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5caa653f-10d0-46a2-81cc-01cb3798075e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7269c6ca-e946-40a5-ac8b-c5ef060b09ff" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BF13B1C-38D3-42D6-8A5C-6D31028437EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
+    <ds:schemaRef ds:uri="7269c6ca-e946-40a5-ac8b-c5ef060b09ff"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07060BB5-5F94-4742-B93F-B4D1C211ED2E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -33893,23 +36002,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90557570-2947-467E-9F2E-D83CEC05A5B9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BF13B1C-38D3-42D6-8A5C-6D31028437EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5caa653f-10d0-46a2-81cc-01cb3798075e"/>
-    <ds:schemaRef ds:uri="7269c6ca-e946-40a5-ac8b-c5ef060b09ff"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
2 steg frem, 1 tilbake
</commit_message>
<xml_diff>
--- a/Input_data_testkode.xlsx
+++ b/Input_data_testkode.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b737bfa27afa4358/Dokumenter/10. semester/Til master/Master_multi_stage_v1-2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="14_{09171854-F596-4674-B3FD-25D610E752C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AB7C96D6-C254-48DA-919C-01CAD67B8B96}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="14_{09171854-F596-4674-B3FD-25D610E752C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0FDB9FF4-C618-424F-AB52-6AA7187B6223}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="40" activeTab="48" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="49" activeTab="58" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Par_ActivationFactor_Dwn_Reg" sheetId="1" r:id="rId1"/>
@@ -49,30 +49,31 @@
     <sheet name="Set_of_FlexibleLoadForEC" sheetId="32" r:id="rId34"/>
     <sheet name="Set_of_Month" sheetId="33" r:id="rId35"/>
     <sheet name="Set_of_Nodes" sheetId="34" r:id="rId36"/>
-    <sheet name="Set_of_Technology" sheetId="35" r:id="rId37"/>
-    <sheet name="Set_of_TimeSteps" sheetId="36" r:id="rId38"/>
-    <sheet name="Subset_LoadShiftWindow" sheetId="37" r:id="rId39"/>
-    <sheet name="Set_of_LoadShiftingInterval" sheetId="46" r:id="rId40"/>
-    <sheet name="Subset_of_TimeStepsInMonth" sheetId="38" r:id="rId41"/>
-    <sheet name="Subset_ShiftableLoadForEC" sheetId="47" r:id="rId42"/>
-    <sheet name="Subset_ECToTech" sheetId="40" r:id="rId43"/>
-    <sheet name="Subset_TechToEC" sheetId="41" r:id="rId44"/>
-    <sheet name="Set_Parent_Node" sheetId="51" r:id="rId45"/>
-    <sheet name="Set_parent_coupling" sheetId="52" r:id="rId46"/>
-    <sheet name="Subset_Plan_Nodes" sheetId="48" r:id="rId47"/>
-    <sheet name="Subset_ID_Nodes" sheetId="49" r:id="rId48"/>
-    <sheet name="Subset_RT_Nodes" sheetId="50" r:id="rId49"/>
-    <sheet name="Set_Mode_of_Operation" sheetId="53" r:id="rId50"/>
-    <sheet name="Par_BatteryCost" sheetId="55" r:id="rId51"/>
-    <sheet name="Par_CostImbalance" sheetId="56" r:id="rId52"/>
-    <sheet name="Par_SpotPrice" sheetId="57" r:id="rId53"/>
-    <sheet name="Par_IntradayPrice" sheetId="58" r:id="rId54"/>
-    <sheet name="Par_RK_UpPrice" sheetId="59" r:id="rId55"/>
-    <sheet name="Par_RK_DwnPrice" sheetId="60" r:id="rId56"/>
-    <sheet name="Set_Strategic_Periods" sheetId="54" r:id="rId57"/>
-    <sheet name="Par_Max_Capex_tec" sheetId="61" r:id="rId58"/>
-    <sheet name="Par_Max_Capex_bat" sheetId="62" r:id="rId59"/>
-    <sheet name="Par_Max_Carbon_Emission" sheetId="63" r:id="rId60"/>
+    <sheet name="Par_Ramping_factor" sheetId="64" r:id="rId37"/>
+    <sheet name="Set_of_Technology" sheetId="35" r:id="rId38"/>
+    <sheet name="Set_of_TimeSteps" sheetId="36" r:id="rId39"/>
+    <sheet name="Subset_LoadShiftWindow" sheetId="37" r:id="rId40"/>
+    <sheet name="Set_of_LoadShiftingInterval" sheetId="46" r:id="rId41"/>
+    <sheet name="Subset_of_TimeStepsInMonth" sheetId="38" r:id="rId42"/>
+    <sheet name="Subset_ShiftableLoadForEC" sheetId="47" r:id="rId43"/>
+    <sheet name="Subset_ECToTech" sheetId="40" r:id="rId44"/>
+    <sheet name="Subset_TechToEC" sheetId="41" r:id="rId45"/>
+    <sheet name="Set_Parent_Node" sheetId="51" r:id="rId46"/>
+    <sheet name="Set_parent_coupling" sheetId="52" r:id="rId47"/>
+    <sheet name="Subset_Plan_Nodes" sheetId="48" r:id="rId48"/>
+    <sheet name="Subset_ID_Nodes" sheetId="49" r:id="rId49"/>
+    <sheet name="Subset_RT_Nodes" sheetId="50" r:id="rId50"/>
+    <sheet name="Set_Mode_of_Operation" sheetId="53" r:id="rId51"/>
+    <sheet name="Par_BatteryCost" sheetId="55" r:id="rId52"/>
+    <sheet name="Par_CostImbalance" sheetId="56" r:id="rId53"/>
+    <sheet name="Par_SpotPrice" sheetId="57" r:id="rId54"/>
+    <sheet name="Par_IntradayPrice" sheetId="58" r:id="rId55"/>
+    <sheet name="Par_RK_UpPrice" sheetId="59" r:id="rId56"/>
+    <sheet name="Par_RK_DwnPrice" sheetId="60" r:id="rId57"/>
+    <sheet name="Set_Strategic_Periods" sheetId="54" r:id="rId58"/>
+    <sheet name="Par_Max_Capex_tec" sheetId="61" r:id="rId59"/>
+    <sheet name="Par_Max_Capex_bat" sheetId="62" r:id="rId60"/>
+    <sheet name="Par_Max_Carbon_Emission" sheetId="63" r:id="rId61"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">Par_ExportCost!$A$3:$D$59</definedName>
@@ -96,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2126" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2139" uniqueCount="138">
   <si>
     <t>Benevning:</t>
   </si>
@@ -845,6 +846,9 @@
   <si>
     <t>RKDwnPrice</t>
   </si>
+  <si>
+    <t>Ramping factor</t>
+  </si>
 </sst>
 </file>
 
@@ -1493,7 +1497,7 @@
       </c>
       <c r="C4" s="11">
         <f ca="1">RANDBETWEEN(0,1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1541,7 +1545,7 @@
       </c>
       <c r="C8" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1613,7 +1617,7 @@
       </c>
       <c r="C14" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1625,7 +1629,7 @@
       </c>
       <c r="C15" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1637,7 +1641,7 @@
       </c>
       <c r="C16" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1649,7 +1653,7 @@
       </c>
       <c r="C17" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1661,7 +1665,7 @@
       </c>
       <c r="C18" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1697,7 +1701,7 @@
       </c>
       <c r="C21" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1721,7 +1725,7 @@
       </c>
       <c r="C23" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1733,7 +1737,7 @@
       </c>
       <c r="C24" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1745,7 +1749,7 @@
       </c>
       <c r="C25" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1757,7 +1761,7 @@
       </c>
       <c r="C26" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1769,7 +1773,7 @@
       </c>
       <c r="C27" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1781,7 +1785,7 @@
       </c>
       <c r="C28" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1793,7 +1797,7 @@
       </c>
       <c r="C29" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1805,7 +1809,7 @@
       </c>
       <c r="C30" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1817,7 +1821,7 @@
       </c>
       <c r="C31" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1877,7 +1881,7 @@
       </c>
       <c r="C36" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1889,7 +1893,7 @@
       </c>
       <c r="C37" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1961,7 +1965,7 @@
       </c>
       <c r="C43" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1973,7 +1977,7 @@
       </c>
       <c r="C44" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1985,7 +1989,7 @@
       </c>
       <c r="C45" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -2009,7 +2013,7 @@
       </c>
       <c r="C47" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -14654,7 +14658,7 @@
       </c>
       <c r="C4" s="11">
         <f ca="1">RANDBETWEEN(0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -14666,7 +14670,7 @@
       </c>
       <c r="C5" s="11">
         <f t="shared" ref="C5:C48" ca="1" si="0">RANDBETWEEN(0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -14678,7 +14682,7 @@
       </c>
       <c r="C6" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -14690,7 +14694,7 @@
       </c>
       <c r="C7" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -14714,7 +14718,7 @@
       </c>
       <c r="C9" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -14738,7 +14742,7 @@
       </c>
       <c r="C11" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -14750,7 +14754,7 @@
       </c>
       <c r="C12" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -14762,7 +14766,7 @@
       </c>
       <c r="C13" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -14774,7 +14778,7 @@
       </c>
       <c r="C14" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -14786,7 +14790,7 @@
       </c>
       <c r="C15" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -14810,7 +14814,7 @@
       </c>
       <c r="C17" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -14846,7 +14850,7 @@
       </c>
       <c r="C20" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -14870,7 +14874,7 @@
       </c>
       <c r="C22" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -14906,7 +14910,7 @@
       </c>
       <c r="C25" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -14930,7 +14934,7 @@
       </c>
       <c r="C27" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -14942,7 +14946,7 @@
       </c>
       <c r="C28" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -14954,7 +14958,7 @@
       </c>
       <c r="C29" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -14966,7 +14970,7 @@
       </c>
       <c r="C30" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -14978,7 +14982,7 @@
       </c>
       <c r="C31" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -14990,7 +14994,7 @@
       </c>
       <c r="C32" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -15014,7 +15018,7 @@
       </c>
       <c r="C34" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -15026,7 +15030,7 @@
       </c>
       <c r="C35" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -15062,7 +15066,7 @@
       </c>
       <c r="C38" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -15086,7 +15090,7 @@
       </c>
       <c r="C40" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -15110,7 +15114,7 @@
       </c>
       <c r="C42" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -15146,7 +15150,7 @@
       </c>
       <c r="C45" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -15158,7 +15162,7 @@
       </c>
       <c r="C46" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -15170,7 +15174,7 @@
       </c>
       <c r="C47" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -20522,7 +20526,7 @@
       </c>
       <c r="C4" s="28">
         <f ca="1">RANDBETWEEN(0,30)</f>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -20534,7 +20538,7 @@
       </c>
       <c r="C5" s="28">
         <f t="shared" ref="C5:C48" ca="1" si="0">RANDBETWEEN(0,30)</f>
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -20546,7 +20550,7 @@
       </c>
       <c r="C6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -20558,7 +20562,7 @@
       </c>
       <c r="C7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>23</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -20570,7 +20574,7 @@
       </c>
       <c r="C8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -20582,7 +20586,7 @@
       </c>
       <c r="C9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -20594,7 +20598,7 @@
       </c>
       <c r="C10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -20606,7 +20610,7 @@
       </c>
       <c r="C11" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -20618,7 +20622,7 @@
       </c>
       <c r="C12" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -20630,7 +20634,7 @@
       </c>
       <c r="C13" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -20642,7 +20646,7 @@
       </c>
       <c r="C14" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -20654,7 +20658,7 @@
       </c>
       <c r="C15" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>28</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -20666,7 +20670,7 @@
       </c>
       <c r="C16" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -20678,7 +20682,7 @@
       </c>
       <c r="C17" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -20690,7 +20694,7 @@
       </c>
       <c r="C18" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -20702,7 +20706,7 @@
       </c>
       <c r="C19" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -20714,7 +20718,7 @@
       </c>
       <c r="C20" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -20726,7 +20730,7 @@
       </c>
       <c r="C21" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -20738,7 +20742,7 @@
       </c>
       <c r="C22" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -20750,7 +20754,7 @@
       </c>
       <c r="C23" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>23</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -20762,7 +20766,7 @@
       </c>
       <c r="C24" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -20774,7 +20778,7 @@
       </c>
       <c r="C25" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D25" s="3"/>
     </row>
@@ -20787,7 +20791,7 @@
       </c>
       <c r="C26" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -20799,7 +20803,7 @@
       </c>
       <c r="C27" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -20811,7 +20815,7 @@
       </c>
       <c r="C28" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -20823,7 +20827,7 @@
       </c>
       <c r="C29" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -20847,7 +20851,7 @@
       </c>
       <c r="C31" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -20859,7 +20863,7 @@
       </c>
       <c r="C32" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -20871,7 +20875,7 @@
       </c>
       <c r="C33" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -20883,7 +20887,7 @@
       </c>
       <c r="C34" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+        <v>13</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -20895,7 +20899,7 @@
       </c>
       <c r="C35" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>29</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -20907,7 +20911,7 @@
       </c>
       <c r="C36" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -20919,7 +20923,7 @@
       </c>
       <c r="C37" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -20931,7 +20935,7 @@
       </c>
       <c r="C38" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -20955,7 +20959,7 @@
       </c>
       <c r="C40" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -20967,7 +20971,7 @@
       </c>
       <c r="C41" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -20979,7 +20983,7 @@
       </c>
       <c r="C42" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>23</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -20991,7 +20995,7 @@
       </c>
       <c r="C43" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -21003,7 +21007,7 @@
       </c>
       <c r="C44" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -21015,7 +21019,7 @@
       </c>
       <c r="C45" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>28</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -21027,7 +21031,7 @@
       </c>
       <c r="C46" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -21039,7 +21043,7 @@
       </c>
       <c r="C47" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>24</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -21051,7 +21055,7 @@
       </c>
       <c r="C48" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -22014,11 +22018,125 @@
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02BC2358-B737-4B12-BCF2-983233884487}">
+  <dimension ref="A3:B14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>125</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
   <dimension ref="A3:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="A4" sqref="A4:A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22116,7 +22234,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
   <dimension ref="A3:A6"/>
   <sheetViews>
@@ -22143,49 +22261,6 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
-  <dimension ref="A3:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
         <v>3</v>
       </c>
     </row>
@@ -22250,7 +22325,7 @@
       </c>
       <c r="C4" s="28">
         <f ca="1">RANDBETWEEN(0,30)</f>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H4" s="32"/>
       <c r="I4" s="32"/>
@@ -22269,7 +22344,7 @@
       </c>
       <c r="C5" s="28">
         <f t="shared" ref="C5:C48" ca="1" si="0">RANDBETWEEN(0,30)</f>
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="H5" s="32"/>
       <c r="I5" s="34"/>
@@ -22288,7 +22363,7 @@
       </c>
       <c r="C6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="H6" s="32"/>
       <c r="I6" s="34"/>
@@ -22307,7 +22382,7 @@
       </c>
       <c r="C7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="H7" s="32"/>
       <c r="I7" s="34"/>
@@ -22326,7 +22401,7 @@
       </c>
       <c r="C8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="H8" s="32"/>
       <c r="I8" s="34"/>
@@ -22345,7 +22420,7 @@
       </c>
       <c r="C9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="H9" s="32"/>
       <c r="I9" s="34"/>
@@ -22364,7 +22439,7 @@
       </c>
       <c r="C10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="H10" s="32"/>
       <c r="I10" s="34"/>
@@ -22383,7 +22458,7 @@
       </c>
       <c r="C11" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="H11" s="32"/>
       <c r="I11" s="34"/>
@@ -22402,7 +22477,7 @@
       </c>
       <c r="C12" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="H12" s="32"/>
       <c r="I12" s="34"/>
@@ -22421,7 +22496,7 @@
       </c>
       <c r="C13" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="H13" s="32"/>
       <c r="I13" s="34"/>
@@ -22459,7 +22534,7 @@
       </c>
       <c r="C15" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="H15" s="32"/>
       <c r="I15" s="34"/>
@@ -22478,7 +22553,7 @@
       </c>
       <c r="C16" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="H16" s="32"/>
       <c r="I16" s="34"/>
@@ -22497,7 +22572,7 @@
       </c>
       <c r="C17" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="H17" s="32"/>
       <c r="I17" s="34"/>
@@ -22516,7 +22591,7 @@
       </c>
       <c r="C18" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="H18" s="32"/>
       <c r="I18" s="34"/>
@@ -22535,7 +22610,7 @@
       </c>
       <c r="C19" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="H19" s="32"/>
       <c r="I19" s="34"/>
@@ -22554,7 +22629,7 @@
       </c>
       <c r="C20" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="H20" s="32"/>
       <c r="I20" s="34"/>
@@ -22573,7 +22648,7 @@
       </c>
       <c r="C21" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="H21" s="32"/>
       <c r="I21" s="34"/>
@@ -22592,7 +22667,7 @@
       </c>
       <c r="C22" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="H22" s="32"/>
       <c r="I22" s="34"/>
@@ -22611,7 +22686,7 @@
       </c>
       <c r="C23" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="H23" s="32"/>
       <c r="I23" s="34"/>
@@ -22630,7 +22705,7 @@
       </c>
       <c r="C24" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H24" s="32"/>
       <c r="I24" s="34"/>
@@ -22668,7 +22743,7 @@
       </c>
       <c r="C26" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="H26" s="32"/>
       <c r="I26" s="34"/>
@@ -22687,7 +22762,7 @@
       </c>
       <c r="C27" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H27" s="32"/>
       <c r="I27" s="34"/>
@@ -22706,7 +22781,7 @@
       </c>
       <c r="C28" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="H28" s="32"/>
       <c r="I28" s="33"/>
@@ -22725,7 +22800,7 @@
       </c>
       <c r="C29" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
@@ -22743,7 +22818,7 @@
       </c>
       <c r="C30" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
@@ -22761,7 +22836,7 @@
       </c>
       <c r="C31" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
@@ -22779,7 +22854,7 @@
       </c>
       <c r="C32" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
@@ -22797,7 +22872,7 @@
       </c>
       <c r="C33" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
@@ -22815,7 +22890,7 @@
       </c>
       <c r="C34" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
@@ -22833,7 +22908,7 @@
       </c>
       <c r="C35" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
@@ -22851,7 +22926,7 @@
       </c>
       <c r="C36" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
@@ -22863,7 +22938,7 @@
       </c>
       <c r="C37" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
@@ -22875,7 +22950,7 @@
       </c>
       <c r="C38" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
@@ -22887,7 +22962,7 @@
       </c>
       <c r="C39" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
@@ -22899,7 +22974,7 @@
       </c>
       <c r="C40" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+        <v>9</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
@@ -22911,7 +22986,7 @@
       </c>
       <c r="C41" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
@@ -22923,7 +22998,7 @@
       </c>
       <c r="C42" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
@@ -22935,7 +23010,7 @@
       </c>
       <c r="C43" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+        <v>9</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
@@ -22947,7 +23022,7 @@
       </c>
       <c r="C44" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+        <v>18</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
@@ -22959,7 +23034,7 @@
       </c>
       <c r="C45" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
@@ -22971,7 +23046,7 @@
       </c>
       <c r="C46" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
@@ -22983,7 +23058,7 @@
       </c>
       <c r="C47" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
@@ -22995,7 +23070,7 @@
       </c>
       <c r="C48" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -23004,6 +23079,49 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
+  <dimension ref="A3:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D2573C2-678A-8345-B842-4FD1416ECFA0}">
   <dimension ref="A3:A4"/>
   <sheetViews>
@@ -23028,7 +23146,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
   <dimension ref="A3:A6"/>
   <sheetViews>
@@ -23066,7 +23184,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F9D7F70-69FF-DE4A-BA10-E984F41A10EA}">
   <dimension ref="A3:B9"/>
   <sheetViews>
@@ -23140,7 +23258,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
   <dimension ref="A3:C22"/>
   <sheetViews>
@@ -23343,7 +23461,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
   <dimension ref="A3:I46"/>
   <sheetViews>
@@ -23687,7 +23805,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{878D8E24-3762-4CAA-87A5-76A089DCF7E4}">
   <dimension ref="A3:A10"/>
   <sheetViews>
@@ -23745,7 +23863,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7640134B-DB60-42C6-A2E8-04D6D42E9B9A}">
   <dimension ref="A3:B17"/>
   <sheetViews>
@@ -23880,12 +23998,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28660982-5EEB-48E8-93DD-AAB15376230B}">
   <dimension ref="A3:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:J17"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23894,7 +24012,7 @@
       <c r="A3" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="8" t="s">
         <v>115</v>
       </c>
     </row>
@@ -23919,7 +24037,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FC82373-EEE5-4EA7-B1F0-86A1D4B373B0}">
   <dimension ref="A3:B7"/>
   <sheetViews>
@@ -23971,96 +24089,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF942341-9D13-4514-BD96-A0AB2FEC6496}">
-  <dimension ref="A3:J11"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>8</v>
-      </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>9</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>10</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>11</v>
-      </c>
-      <c r="B7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>12</v>
-      </c>
-      <c r="B8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>13</v>
-      </c>
-      <c r="B9">
-        <v>6</v>
-      </c>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>14</v>
-      </c>
-      <c r="B10">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>15</v>
-      </c>
-      <c r="B11">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -24117,7 +24145,7 @@
       </c>
       <c r="C4" s="28">
         <f ca="1">RANDBETWEEN(0,30)</f>
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
@@ -24140,7 +24168,7 @@
       </c>
       <c r="C5" s="28">
         <f t="shared" ref="C5:C48" ca="1" si="0">RANDBETWEEN(0,30)</f>
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
@@ -24163,7 +24191,7 @@
       </c>
       <c r="C6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
@@ -24186,7 +24214,7 @@
       </c>
       <c r="C7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
@@ -24209,7 +24237,7 @@
       </c>
       <c r="C8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
@@ -24232,7 +24260,7 @@
       </c>
       <c r="C9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
@@ -24255,7 +24283,7 @@
       </c>
       <c r="C10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
@@ -24278,7 +24306,7 @@
       </c>
       <c r="C11" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
@@ -24301,7 +24329,7 @@
       </c>
       <c r="C12" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
@@ -24324,7 +24352,7 @@
       </c>
       <c r="C13" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
@@ -24347,7 +24375,7 @@
       </c>
       <c r="C14" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
@@ -24370,7 +24398,7 @@
       </c>
       <c r="C15" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
@@ -24393,7 +24421,7 @@
       </c>
       <c r="C16" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
@@ -24416,7 +24444,7 @@
       </c>
       <c r="C17" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
@@ -24439,7 +24467,7 @@
       </c>
       <c r="C18" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
@@ -24462,7 +24490,7 @@
       </c>
       <c r="C19" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
@@ -24485,7 +24513,7 @@
       </c>
       <c r="C20" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
@@ -24508,7 +24536,7 @@
       </c>
       <c r="C21" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
@@ -24531,7 +24559,7 @@
       </c>
       <c r="C22" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
@@ -24554,7 +24582,7 @@
       </c>
       <c r="C23" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
@@ -24577,7 +24605,7 @@
       </c>
       <c r="C24" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
@@ -24600,7 +24628,7 @@
       </c>
       <c r="C25" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
@@ -24623,7 +24651,7 @@
       </c>
       <c r="C26" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
@@ -24646,7 +24674,7 @@
       </c>
       <c r="C27" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="E27" s="5"/>
       <c r="H27" s="5"/>
@@ -24670,7 +24698,7 @@
       </c>
       <c r="C28" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
@@ -24693,7 +24721,7 @@
       </c>
       <c r="C29" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
@@ -24716,7 +24744,7 @@
       </c>
       <c r="C30" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
@@ -24739,7 +24767,7 @@
       </c>
       <c r="C31" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
@@ -24762,7 +24790,7 @@
       </c>
       <c r="C32" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
@@ -24785,7 +24813,7 @@
       </c>
       <c r="C33" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
@@ -24808,7 +24836,7 @@
       </c>
       <c r="C34" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
@@ -24831,7 +24859,7 @@
       </c>
       <c r="C35" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
@@ -24843,7 +24871,7 @@
       </c>
       <c r="C36" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
@@ -24855,7 +24883,7 @@
       </c>
       <c r="C37" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
@@ -24867,7 +24895,7 @@
       </c>
       <c r="C38" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
@@ -24879,7 +24907,7 @@
       </c>
       <c r="C39" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
@@ -24891,7 +24919,7 @@
       </c>
       <c r="C40" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
@@ -24903,7 +24931,7 @@
       </c>
       <c r="C41" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>24</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
@@ -24915,7 +24943,7 @@
       </c>
       <c r="C42" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>30</v>
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
@@ -24927,7 +24955,7 @@
       </c>
       <c r="C43" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>26</v>
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
@@ -24939,7 +24967,7 @@
       </c>
       <c r="C44" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
@@ -24951,7 +24979,7 @@
       </c>
       <c r="C45" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+        <v>11</v>
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
@@ -24963,7 +24991,7 @@
       </c>
       <c r="C46" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
@@ -24975,7 +25003,7 @@
       </c>
       <c r="C47" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
@@ -24987,7 +25015,7 @@
       </c>
       <c r="C48" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -24996,6 +25024,96 @@
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF942341-9D13-4514-BD96-A0AB2FEC6496}">
+  <dimension ref="A3:J11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{061BAE23-20C3-402A-8365-5ED2D9265339}">
   <dimension ref="A3:A9"/>
   <sheetViews>
@@ -25048,7 +25166,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7815BD0D-D4C8-43C3-B5E1-419A131BCC6A}">
   <dimension ref="A3:B16"/>
   <sheetViews>
@@ -25178,7 +25296,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B076616-024E-4AB1-B79B-88202D242CCF}">
   <dimension ref="A3:A4"/>
   <sheetViews>
@@ -25207,7 +25325,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84C73887-EC92-4CCB-BB63-90308D4E3D86}">
   <dimension ref="A3:C48"/>
   <sheetViews>
@@ -25749,7 +25867,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A34583D8-B68B-48CF-AB50-5E1E48B2C8C1}">
   <dimension ref="A3:C48"/>
   <sheetViews>
@@ -26291,7 +26409,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE259879-7F8E-4068-80DD-1A71A9A2E767}">
   <dimension ref="A3:C48"/>
   <sheetViews>
@@ -26833,7 +26951,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E77D990-D668-4B4C-BC47-633A78174A57}">
   <dimension ref="A3:C48"/>
   <sheetViews>
@@ -27375,7 +27493,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFD6BE9E-879D-4B2B-94E0-B0F968CE8029}">
   <dimension ref="A3:A4"/>
   <sheetViews>
@@ -27400,12 +27518,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79D8A7B4-563D-4ED3-B0E1-BBA90E6A0CD9}">
   <dimension ref="A3:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27506,136 +27624,6 @@
         <v>19</v>
       </c>
       <c r="B14">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43D2A640-3DE1-4626-909C-0B031DDA6CF5}">
-  <dimension ref="A3:B16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>98</v>
-      </c>
-      <c r="B11">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>99</v>
-      </c>
-      <c r="B12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>100</v>
-      </c>
-      <c r="B13">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>101</v>
-      </c>
-      <c r="B14">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>102</v>
-      </c>
-      <c r="B15">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>103</v>
-      </c>
-      <c r="B16">
         <v>5</v>
       </c>
     </row>
@@ -27694,7 +27682,7 @@
       </c>
       <c r="C4" s="28">
         <f ca="1">RANDBETWEEN(0,30)</f>
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -27706,7 +27694,7 @@
       </c>
       <c r="C5" s="28">
         <f t="shared" ref="C5:C48" ca="1" si="0">RANDBETWEEN(0,30)</f>
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -27718,7 +27706,7 @@
       </c>
       <c r="C6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -27730,7 +27718,7 @@
       </c>
       <c r="C7" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -27742,7 +27730,7 @@
       </c>
       <c r="C8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -27754,7 +27742,7 @@
       </c>
       <c r="C9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -27766,7 +27754,7 @@
       </c>
       <c r="C10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>28</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -27778,7 +27766,7 @@
       </c>
       <c r="C11" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -27790,7 +27778,7 @@
       </c>
       <c r="C12" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>23</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -27802,7 +27790,7 @@
       </c>
       <c r="C13" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -27814,7 +27802,7 @@
       </c>
       <c r="C14" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -27838,7 +27826,7 @@
       </c>
       <c r="C16" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -27850,7 +27838,7 @@
       </c>
       <c r="C17" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -27862,7 +27850,7 @@
       </c>
       <c r="C18" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -27874,7 +27862,7 @@
       </c>
       <c r="C19" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -27886,7 +27874,7 @@
       </c>
       <c r="C20" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -27898,7 +27886,7 @@
       </c>
       <c r="C21" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -27910,7 +27898,7 @@
       </c>
       <c r="C22" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -27922,7 +27910,7 @@
       </c>
       <c r="C23" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -27934,7 +27922,7 @@
       </c>
       <c r="C24" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -27946,7 +27934,7 @@
       </c>
       <c r="C25" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -27958,7 +27946,7 @@
       </c>
       <c r="C26" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -27970,7 +27958,7 @@
       </c>
       <c r="C27" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -27982,7 +27970,7 @@
       </c>
       <c r="C28" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>28</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -27994,7 +27982,7 @@
       </c>
       <c r="C29" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -28006,7 +27994,7 @@
       </c>
       <c r="C30" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -28018,7 +28006,7 @@
       </c>
       <c r="C31" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -28030,7 +28018,7 @@
       </c>
       <c r="C32" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -28042,7 +28030,7 @@
       </c>
       <c r="C33" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -28054,7 +28042,7 @@
       </c>
       <c r="C34" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>24</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -28066,7 +28054,7 @@
       </c>
       <c r="C35" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -28078,7 +28066,7 @@
       </c>
       <c r="C36" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -28090,7 +28078,7 @@
       </c>
       <c r="C37" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -28102,7 +28090,7 @@
       </c>
       <c r="C38" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -28114,7 +28102,7 @@
       </c>
       <c r="C39" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -28126,7 +28114,7 @@
       </c>
       <c r="C40" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -28138,7 +28126,7 @@
       </c>
       <c r="C41" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -28150,7 +28138,7 @@
       </c>
       <c r="C42" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -28162,7 +28150,7 @@
       </c>
       <c r="C43" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -28174,7 +28162,7 @@
       </c>
       <c r="C44" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -28186,7 +28174,7 @@
       </c>
       <c r="C45" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -28198,7 +28186,7 @@
       </c>
       <c r="C46" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -28210,7 +28198,7 @@
       </c>
       <c r="C47" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -28222,7 +28210,7 @@
       </c>
       <c r="C48" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -28231,6 +28219,136 @@
 </file>
 
 <file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43D2A640-3DE1-4626-909C-0B031DDA6CF5}">
+  <dimension ref="A3:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>101</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>102</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>103</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02D11E0E-41D4-4644-84B7-5D54908DADEE}">
   <dimension ref="A3:A4"/>
   <sheetViews>

</xml_diff>